<commit_message>
2023/03/21 서정현/ DB 수정
</commit_message>
<xml_diff>
--- a/DB/LeMo 테이블 명세서 v1.0.xlsx
+++ b/DB/LeMo 테이블 명세서 v1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java2\Desktop\workspace\LeMo\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ooo33.DESKTOP-56U45AS\Desktop\workspace\LeMo\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC3F3F-EC34-46CF-B347-320D59B674AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4395" windowWidth="29040" windowHeight="15840" tabRatio="996" firstSheet="4" activeTab="22"/>
+    <workbookView xWindow="-28920" yWindow="-4395" windowWidth="29040" windowHeight="15840" tabRatio="996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="테이블" sheetId="1" r:id="rId1"/>
@@ -42,7 +43,7 @@
     <sheet name="좋아요" sheetId="36" r:id="rId28"/>
     <sheet name="나의 찜" sheetId="38" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="595">
   <si>
     <t>작업일자</t>
   </si>
@@ -2978,11 +2979,23 @@
     <t xml:space="preserve"> lemo_product_qna(판매자 문의) &gt; pQna_title 컬럼 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>pQna_reply_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의 답변일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> lemo_product_qna(판매자 문의) &gt; pQna_reply_date 컬럼 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -4261,13 +4274,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4276,59 +4286,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -4341,6 +4312,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4387,20 +4373,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4410,6 +4429,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4423,26 +4445,17 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4709,361 +4722,361 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1012"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H14" sqref="H14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="5" customWidth="1"/>
-    <col min="2" max="3" width="6.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" customWidth="1"/>
-    <col min="7" max="8" width="7.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="6.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="5" customWidth="1"/>
+    <col min="7" max="8" width="7.44140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="17" style="5" customWidth="1"/>
-    <col min="10" max="27" width="7.5703125" style="5" customWidth="1"/>
-    <col min="28" max="16384" width="14.42578125" style="5"/>
+    <col min="10" max="27" width="7.5546875" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="4.5" customHeight="1"/>
     <row r="2" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="134"/>
       <c r="F2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="113"/>
-      <c r="I2" s="114"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="115"/>
     </row>
     <row r="3" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B3" s="109"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
       <c r="F3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="112" t="s">
+      <c r="G3" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="113"/>
-      <c r="I3" s="114"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="115"/>
     </row>
     <row r="4" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="114"/>
-      <c r="D4" s="112" t="s">
+      <c r="C4" s="115"/>
+      <c r="D4" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="114"/>
+      <c r="E4" s="115"/>
       <c r="F4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="116">
+      <c r="G4" s="140">
         <v>44982</v>
       </c>
-      <c r="H4" s="113"/>
-      <c r="I4" s="114"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="115"/>
     </row>
     <row r="5" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="112" t="s">
+      <c r="C5" s="115"/>
+      <c r="D5" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="114"/>
+      <c r="E5" s="115"/>
       <c r="F5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="112" t="s">
+      <c r="G5" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="113"/>
-      <c r="I5" s="114"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="115"/>
     </row>
     <row r="6" spans="2:9" ht="6" customHeight="1"/>
     <row r="7" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="121" t="s">
+      <c r="C7" s="139"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="113"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="121" t="s">
+      <c r="F7" s="139"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="114"/>
+      <c r="I7" s="115"/>
     </row>
     <row r="8" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="108" t="s">
         <v>382</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="125" t="s">
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="111" t="s">
         <v>554</v>
       </c>
-      <c r="F8" s="123"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="113"/>
     </row>
     <row r="9" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="125" t="s">
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="111" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="105"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="113"/>
     </row>
     <row r="10" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="118"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="101" t="s">
+      <c r="C10" s="106"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="100"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="105"/>
     </row>
     <row r="11" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="101" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="103" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="100"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="105"/>
     </row>
     <row r="12" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="100" t="s">
         <v>515</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="101" t="s">
+      <c r="C12" s="106"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="118"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="100"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="105"/>
     </row>
     <row r="13" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="100" t="s">
         <v>516</v>
       </c>
-      <c r="C13" s="118"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="101" t="s">
+      <c r="C13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="103" t="s">
         <v>517</v>
       </c>
-      <c r="F13" s="118"/>
-      <c r="G13" s="119"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="100"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="105"/>
     </row>
     <row r="14" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="101" t="s">
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="100"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="105"/>
     </row>
     <row r="15" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="100" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="101" t="s">
+      <c r="C15" s="101"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="103" t="s">
         <v>246</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="100"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="105"/>
     </row>
     <row r="16" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B16" s="117" t="s">
+      <c r="B16" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="C16" s="102"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="101" t="s">
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="103" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="102"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="100"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="105"/>
     </row>
     <row r="17" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="102"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="101" t="s">
+      <c r="C17" s="101"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="103" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="100"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="105"/>
     </row>
     <row r="18" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="101" t="s">
+      <c r="C18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103" t="s">
         <v>249</v>
       </c>
-      <c r="F18" s="102"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="100"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="105"/>
     </row>
     <row r="19" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="100" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="102"/>
-      <c r="D19" s="103"/>
-      <c r="E19" s="101" t="s">
+      <c r="C19" s="101"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="103" t="s">
         <v>472</v>
       </c>
-      <c r="F19" s="102"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="100"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="105"/>
     </row>
     <row r="20" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B20" s="117" t="s">
+      <c r="B20" s="100" t="s">
         <v>477</v>
       </c>
-      <c r="C20" s="102"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="101" t="s">
+      <c r="C20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="103" t="s">
         <v>476</v>
       </c>
-      <c r="F20" s="102"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="100"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="105"/>
     </row>
     <row r="21" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="100" t="s">
         <v>415</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="101" t="s">
+      <c r="C21" s="101"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="103" t="s">
         <v>461</v>
       </c>
-      <c r="F21" s="102"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="100"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="105"/>
     </row>
     <row r="22" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="100" t="s">
         <v>466</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="101" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="103" t="s">
         <v>467</v>
       </c>
-      <c r="F22" s="102"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="100"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="105"/>
     </row>
     <row r="23" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="102"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="101" t="s">
+      <c r="C23" s="101"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="103" t="s">
         <v>322</v>
       </c>
-      <c r="F23" s="102"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="100"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="105"/>
     </row>
     <row r="24" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="100" t="s">
         <v>384</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="101" t="s">
+      <c r="C24" s="101"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="103" t="s">
         <v>385</v>
       </c>
-      <c r="F24" s="102"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="100"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="105"/>
     </row>
     <row r="25" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B25" s="117" t="s">
+      <c r="B25" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="C25" s="102"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="101" t="s">
+      <c r="C25" s="101"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="103" t="s">
         <v>383</v>
       </c>
-      <c r="F25" s="102"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="100"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="105"/>
     </row>
     <row r="26" spans="2:9" ht="21.75" customHeight="1">
       <c r="B26" s="82" t="s">
@@ -5071,241 +5084,241 @@
       </c>
       <c r="C26" s="83"/>
       <c r="D26" s="84"/>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="103" t="s">
         <v>386</v>
       </c>
-      <c r="F26" s="102"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="100"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="105"/>
     </row>
     <row r="27" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="100" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="101" t="s">
+      <c r="C27" s="101"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="103" t="s">
         <v>252</v>
       </c>
-      <c r="F27" s="102"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="100"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="105"/>
     </row>
     <row r="28" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="100" t="s">
         <v>389</v>
       </c>
-      <c r="C28" s="102"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="101" t="s">
+      <c r="C28" s="101"/>
+      <c r="D28" s="102"/>
+      <c r="E28" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="F28" s="102"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="100"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="105"/>
     </row>
     <row r="29" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B29" s="117" t="s">
+      <c r="B29" s="100" t="s">
         <v>325</v>
       </c>
-      <c r="C29" s="102"/>
-      <c r="D29" s="103"/>
-      <c r="E29" s="101" t="s">
+      <c r="C29" s="101"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="103" t="s">
         <v>390</v>
       </c>
-      <c r="F29" s="102"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="100"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="105"/>
     </row>
     <row r="30" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B30" s="117" t="s">
+      <c r="B30" s="100" t="s">
         <v>393</v>
       </c>
-      <c r="C30" s="102"/>
-      <c r="D30" s="103"/>
-      <c r="E30" s="101" t="s">
+      <c r="C30" s="101"/>
+      <c r="D30" s="102"/>
+      <c r="E30" s="103" t="s">
         <v>392</v>
       </c>
-      <c r="F30" s="102"/>
-      <c r="G30" s="103"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="100"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="105"/>
     </row>
     <row r="31" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="100" t="s">
         <v>410</v>
       </c>
-      <c r="C31" s="102"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="101" t="s">
+      <c r="C31" s="101"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="103" t="s">
         <v>409</v>
       </c>
-      <c r="F31" s="102"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="100"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="105"/>
     </row>
     <row r="32" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B32" s="117" t="s">
+      <c r="B32" s="100" t="s">
         <v>411</v>
       </c>
-      <c r="C32" s="118"/>
-      <c r="D32" s="119"/>
-      <c r="E32" s="101" t="s">
+      <c r="C32" s="106"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="103" t="s">
         <v>395</v>
       </c>
-      <c r="F32" s="118"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="100"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="107"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="105"/>
     </row>
     <row r="33" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B33" s="117" t="s">
+      <c r="B33" s="100" t="s">
         <v>396</v>
       </c>
-      <c r="C33" s="118"/>
-      <c r="D33" s="119"/>
-      <c r="E33" s="101" t="s">
+      <c r="C33" s="106"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="103" t="s">
         <v>397</v>
       </c>
-      <c r="F33" s="118"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="100"/>
-      <c r="N33" s="141"/>
-      <c r="O33" s="141"/>
-      <c r="P33" s="141"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="105"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="99"/>
+      <c r="P33" s="99"/>
     </row>
     <row r="34" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B34" s="117" t="s">
+      <c r="B34" s="100" t="s">
         <v>398</v>
       </c>
-      <c r="C34" s="118"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="101" t="s">
+      <c r="C34" s="106"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="103" t="s">
         <v>399</v>
       </c>
-      <c r="F34" s="118"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="100"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="107"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="105"/>
     </row>
     <row r="35" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B35" s="117"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="100"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="106"/>
+      <c r="G35" s="107"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="105"/>
     </row>
     <row r="36" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B36" s="117"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="100"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="105"/>
     </row>
     <row r="37" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B37" s="140"/>
-      <c r="C37" s="136"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="135"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="137"/>
-      <c r="H37" s="138"/>
-      <c r="I37" s="139"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="128"/>
+      <c r="E37" s="126"/>
+      <c r="F37" s="127"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="130"/>
     </row>
     <row r="38" spans="2:16" ht="6" customHeight="1"/>
     <row r="39" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="126"/>
-      <c r="D39" s="126"/>
-      <c r="E39" s="126"/>
-      <c r="F39" s="126"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="126"/>
-      <c r="I39" s="127"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="118"/>
     </row>
     <row r="40" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B40" s="128"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="129"/>
-      <c r="E40" s="129"/>
-      <c r="F40" s="129"/>
-      <c r="G40" s="129"/>
-      <c r="H40" s="129"/>
-      <c r="I40" s="130"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="120"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="120"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="121"/>
     </row>
     <row r="41" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B41" s="131"/>
-      <c r="C41" s="129"/>
-      <c r="D41" s="129"/>
-      <c r="E41" s="129"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="129"/>
-      <c r="H41" s="129"/>
-      <c r="I41" s="130"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="121"/>
     </row>
     <row r="42" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B42" s="131"/>
-      <c r="C42" s="129"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="129"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="129"/>
-      <c r="H42" s="129"/>
-      <c r="I42" s="130"/>
+      <c r="B42" s="122"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="121"/>
     </row>
     <row r="43" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B43" s="131"/>
-      <c r="C43" s="129"/>
-      <c r="D43" s="129"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="129"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="130"/>
+      <c r="B43" s="122"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120"/>
+      <c r="G43" s="120"/>
+      <c r="H43" s="120"/>
+      <c r="I43" s="121"/>
     </row>
     <row r="44" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B44" s="131"/>
-      <c r="C44" s="129"/>
-      <c r="D44" s="129"/>
-      <c r="E44" s="129"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="129"/>
-      <c r="H44" s="129"/>
-      <c r="I44" s="130"/>
+      <c r="B44" s="122"/>
+      <c r="C44" s="120"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="120"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="120"/>
+      <c r="I44" s="121"/>
     </row>
     <row r="45" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B45" s="131"/>
-      <c r="C45" s="129"/>
-      <c r="D45" s="129"/>
-      <c r="E45" s="129"/>
-      <c r="F45" s="129"/>
-      <c r="G45" s="129"/>
-      <c r="H45" s="129"/>
-      <c r="I45" s="130"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="120"/>
+      <c r="F45" s="120"/>
+      <c r="G45" s="120"/>
+      <c r="H45" s="120"/>
+      <c r="I45" s="121"/>
     </row>
     <row r="46" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B46" s="132"/>
-      <c r="C46" s="133"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="133"/>
-      <c r="F46" s="133"/>
-      <c r="G46" s="133"/>
-      <c r="H46" s="133"/>
-      <c r="I46" s="134"/>
+      <c r="B46" s="123"/>
+      <c r="C46" s="124"/>
+      <c r="D46" s="124"/>
+      <c r="E46" s="124"/>
+      <c r="F46" s="124"/>
+      <c r="G46" s="124"/>
+      <c r="H46" s="124"/>
+      <c r="I46" s="125"/>
     </row>
     <row r="47" spans="2:16" ht="16.5" customHeight="1">
       <c r="B47" s="5" t="s">
@@ -6279,53 +6292,39 @@
     <row r="1012" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B40:I46"/>
@@ -6350,39 +6349,53 @@
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B31:D31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -6391,25 +6404,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:H998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="14.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -6645,15 +6658,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="127"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="160"/>
@@ -7672,25 +7685,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:H1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="14.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -8048,12 +8061,12 @@
       <c r="B22" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="113"/>
-      <c r="D22" s="113"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="114"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="115"/>
     </row>
     <row r="23" spans="2:8" ht="21.75" customHeight="1">
       <c r="B23" s="160" t="s">
@@ -9113,25 +9126,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:H998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="16.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -9351,15 +9364,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="127"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="160"/>
@@ -10378,25 +10391,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B1:H989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -10598,7 +10611,7 @@
       <c r="G12" s="34"/>
       <c r="H12" s="48"/>
     </row>
-    <row r="13" spans="2:8" ht="22.15" customHeight="1">
+    <row r="13" spans="2:8" ht="22.2" customHeight="1">
       <c r="B13" s="61" t="s">
         <v>230</v>
       </c>
@@ -10838,15 +10851,15 @@
     </row>
     <row r="27" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="28" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="127"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="118"/>
     </row>
     <row r="29" spans="2:8" ht="21.75" customHeight="1">
       <c r="B29" s="26" t="s">
@@ -11861,25 +11874,25 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B1:H979"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -12055,15 +12068,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -13070,25 +13083,25 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B1:H979"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="17.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -13264,15 +13277,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -14279,25 +14292,25 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="B1:H979"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -14433,7 +14446,7 @@
       <c r="G12" s="34"/>
       <c r="H12" s="48"/>
     </row>
-    <row r="13" spans="2:8" ht="22.15" customHeight="1">
+    <row r="13" spans="2:8" ht="22.2" customHeight="1">
       <c r="B13" s="61"/>
       <c r="C13" s="56"/>
       <c r="D13" s="13"/>
@@ -14471,15 +14484,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -15486,25 +15499,25 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="B1:H978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -15681,15 +15694,15 @@
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="17" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B17" s="115" t="s">
+      <c r="B17" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
-      <c r="H17" s="127"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="118"/>
     </row>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
       <c r="B18" s="26"/>
@@ -16696,25 +16709,25 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="B1:H974"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="23.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -16877,15 +16890,15 @@
     </row>
     <row r="12" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="13" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B13" s="115" t="s">
+      <c r="B13" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="126"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
-      <c r="H13" s="127"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="118"/>
     </row>
     <row r="14" spans="2:8" ht="21.75" customHeight="1">
       <c r="B14" s="26"/>
@@ -17892,25 +17905,25 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="B1:H981"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -18188,15 +18201,15 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="127"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="118"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="160" t="s">
@@ -19205,495 +19218,501 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="5" customWidth="1"/>
-    <col min="2" max="3" width="6.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="1.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="53.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="6.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="1.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="53.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="17" style="5" customWidth="1"/>
-    <col min="10" max="27" width="7.5703125" style="5" customWidth="1"/>
-    <col min="28" max="16384" width="14.42578125" style="5"/>
+    <col min="10" max="27" width="7.5546875" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="156" t="s">
         <v>568</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
     </row>
     <row r="2" spans="2:9" ht="6" customHeight="1"/>
     <row r="3" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>569</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="121" t="s">
+      <c r="C3" s="139"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="113"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="121" t="s">
+      <c r="F3" s="139"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="114" t="s">
         <v>570</v>
       </c>
-      <c r="I3" s="114"/>
+      <c r="I3" s="115"/>
     </row>
     <row r="4" spans="2:9" ht="42.6" customHeight="1">
-      <c r="B4" s="156">
+      <c r="B4" s="142">
         <v>1</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="159" t="s">
+      <c r="C4" s="143"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="145" t="s">
         <v>571</v>
       </c>
-      <c r="F4" s="123"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="154">
+      <c r="F4" s="109"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="146">
         <v>44999</v>
       </c>
-      <c r="I4" s="155"/>
+      <c r="I4" s="147"/>
     </row>
     <row r="5" spans="2:9" ht="41.25" customHeight="1">
-      <c r="B5" s="156">
+      <c r="B5" s="142">
         <v>2</v>
       </c>
-      <c r="C5" s="157"/>
-      <c r="D5" s="158"/>
-      <c r="E5" s="159" t="s">
+      <c r="C5" s="143"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="145" t="s">
         <v>573</v>
       </c>
-      <c r="F5" s="123"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="154">
+      <c r="F5" s="109"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="146">
         <v>44999</v>
       </c>
-      <c r="I5" s="155"/>
-    </row>
-    <row r="6" spans="2:9" ht="44.45" customHeight="1">
-      <c r="B6" s="146">
+      <c r="I5" s="147"/>
+    </row>
+    <row r="6" spans="2:9" ht="44.4" customHeight="1">
+      <c r="B6" s="148">
         <v>3</v>
       </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="153" t="s">
+      <c r="C6" s="149"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="151" t="s">
         <v>575</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="154">
+      <c r="F6" s="101"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="146">
         <v>45001</v>
       </c>
-      <c r="I6" s="155"/>
+      <c r="I6" s="147"/>
     </row>
     <row r="7" spans="2:9" ht="69" customHeight="1">
-      <c r="B7" s="146">
+      <c r="B7" s="148">
         <v>4</v>
       </c>
-      <c r="C7" s="149"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="153" t="s">
+      <c r="C7" s="152"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="151" t="s">
         <v>581</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="154">
+      <c r="F7" s="101"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="146">
         <v>45001</v>
       </c>
-      <c r="I7" s="155"/>
+      <c r="I7" s="147"/>
     </row>
     <row r="8" spans="2:9" ht="39.6" customHeight="1">
-      <c r="B8" s="146">
+      <c r="B8" s="148">
         <v>5</v>
       </c>
-      <c r="C8" s="147"/>
-      <c r="D8" s="148"/>
-      <c r="E8" s="153" t="s">
+      <c r="C8" s="149"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="151" t="s">
         <v>582</v>
       </c>
-      <c r="F8" s="118"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="151">
+      <c r="F8" s="106"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="154">
         <v>45002</v>
       </c>
-      <c r="I8" s="152"/>
+      <c r="I8" s="155"/>
     </row>
     <row r="9" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B9" s="146">
+      <c r="B9" s="148">
         <v>6</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="101" t="s">
+      <c r="C9" s="149"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="103" t="s">
         <v>583</v>
       </c>
-      <c r="F9" s="118"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="151">
+      <c r="F9" s="106"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="154">
         <v>45003</v>
       </c>
-      <c r="I9" s="152"/>
+      <c r="I9" s="155"/>
     </row>
     <row r="10" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B10" s="146">
+      <c r="B10" s="148">
         <v>7</v>
       </c>
-      <c r="C10" s="149"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="101" t="s">
+      <c r="C10" s="152"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="103" t="s">
         <v>584</v>
       </c>
-      <c r="F10" s="118"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="151">
+      <c r="F10" s="106"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="154">
         <v>45005</v>
       </c>
-      <c r="I10" s="152"/>
+      <c r="I10" s="155"/>
     </row>
     <row r="11" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B11" s="146">
+      <c r="B11" s="148">
         <v>8</v>
       </c>
-      <c r="C11" s="149"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="101" t="s">
+      <c r="C11" s="152"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="103" t="s">
         <v>590</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="151">
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="154">
         <v>45006</v>
       </c>
-      <c r="I11" s="152"/>
+      <c r="I11" s="155"/>
     </row>
     <row r="12" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B12" s="146">
+      <c r="B12" s="148">
         <v>9</v>
       </c>
-      <c r="C12" s="149"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="101" t="s">
+      <c r="C12" s="152"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="103" t="s">
         <v>591</v>
       </c>
-      <c r="F12" s="102"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="151">
+      <c r="F12" s="101"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="154">
         <v>45006</v>
       </c>
-      <c r="I12" s="152"/>
+      <c r="I12" s="155"/>
     </row>
     <row r="13" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B13" s="146"/>
-      <c r="C13" s="149"/>
-      <c r="D13" s="150"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="100"/>
+      <c r="B13" s="148">
+        <v>10</v>
+      </c>
+      <c r="C13" s="152"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="103" t="s">
+        <v>594</v>
+      </c>
+      <c r="F13" s="101"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="154">
+        <v>45006</v>
+      </c>
+      <c r="I13" s="155"/>
     </row>
     <row r="14" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B14" s="146"/>
-      <c r="C14" s="149"/>
-      <c r="D14" s="150"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="100"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="152"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="105"/>
     </row>
     <row r="15" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B15" s="146"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="100"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="105"/>
     </row>
     <row r="16" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B16" s="146"/>
-      <c r="C16" s="149"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="100"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="105"/>
     </row>
     <row r="17" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B17" s="146"/>
-      <c r="C17" s="149"/>
-      <c r="D17" s="150"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="100"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="105"/>
     </row>
     <row r="18" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B18" s="146"/>
-      <c r="C18" s="149"/>
-      <c r="D18" s="150"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="100"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="152"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="105"/>
     </row>
     <row r="19" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B19" s="146"/>
-      <c r="C19" s="149"/>
-      <c r="D19" s="150"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="100"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="153"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="105"/>
     </row>
     <row r="20" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B20" s="146"/>
-      <c r="C20" s="149"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="100"/>
+      <c r="B20" s="148"/>
+      <c r="C20" s="152"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="105"/>
     </row>
     <row r="21" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B21" s="146"/>
-      <c r="C21" s="149"/>
-      <c r="D21" s="150"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="100"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="105"/>
     </row>
     <row r="22" spans="2:16" ht="21.75" customHeight="1">
       <c r="B22" s="97"/>
       <c r="C22" s="94"/>
       <c r="D22" s="56"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="100"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="105"/>
     </row>
     <row r="23" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B23" s="146"/>
-      <c r="C23" s="149"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="100"/>
+      <c r="B23" s="148"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="105"/>
     </row>
     <row r="24" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B24" s="146"/>
-      <c r="C24" s="149"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="100"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="152"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="105"/>
     </row>
     <row r="25" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B25" s="146"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="100"/>
+      <c r="B25" s="148"/>
+      <c r="C25" s="152"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="105"/>
     </row>
     <row r="26" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B26" s="146"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="150"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="102"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="100"/>
+      <c r="B26" s="148"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="105"/>
     </row>
     <row r="27" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B27" s="146"/>
-      <c r="C27" s="149"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="100"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="105"/>
     </row>
     <row r="28" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B28" s="146"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="100"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="105"/>
     </row>
     <row r="29" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B29" s="146"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="148"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="100"/>
-      <c r="N29" s="141"/>
-      <c r="O29" s="141"/>
-      <c r="P29" s="141"/>
+      <c r="B29" s="148"/>
+      <c r="C29" s="149"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="107"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="105"/>
+      <c r="N29" s="99"/>
+      <c r="O29" s="99"/>
+      <c r="P29" s="99"/>
     </row>
     <row r="30" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B30" s="146"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="100"/>
+      <c r="B30" s="148"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="105"/>
     </row>
     <row r="31" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B31" s="146"/>
-      <c r="C31" s="147"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="100"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="107"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="105"/>
     </row>
     <row r="32" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B32" s="146"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="148"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="100"/>
+      <c r="B32" s="148"/>
+      <c r="C32" s="149"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="107"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="105"/>
     </row>
     <row r="33" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B33" s="142"/>
-      <c r="C33" s="143"/>
-      <c r="D33" s="144"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="138"/>
-      <c r="I33" s="139"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="158"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="127"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="130"/>
     </row>
     <row r="34" spans="2:9" ht="6" customHeight="1"/>
     <row r="35" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B35" s="115" t="s">
+      <c r="B35" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="126"/>
-      <c r="D35" s="126"/>
-      <c r="E35" s="126"/>
-      <c r="F35" s="126"/>
-      <c r="G35" s="126"/>
-      <c r="H35" s="126"/>
-      <c r="I35" s="127"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="118"/>
     </row>
     <row r="36" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B36" s="128"/>
-      <c r="C36" s="129"/>
-      <c r="D36" s="129"/>
-      <c r="E36" s="129"/>
-      <c r="F36" s="129"/>
-      <c r="G36" s="129"/>
-      <c r="H36" s="129"/>
-      <c r="I36" s="130"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="121"/>
     </row>
     <row r="37" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B37" s="131"/>
-      <c r="C37" s="129"/>
-      <c r="D37" s="129"/>
-      <c r="E37" s="129"/>
-      <c r="F37" s="129"/>
-      <c r="G37" s="129"/>
-      <c r="H37" s="129"/>
-      <c r="I37" s="130"/>
+      <c r="B37" s="122"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="120"/>
+      <c r="I37" s="121"/>
     </row>
     <row r="38" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B38" s="131"/>
-      <c r="C38" s="129"/>
-      <c r="D38" s="129"/>
-      <c r="E38" s="129"/>
-      <c r="F38" s="129"/>
-      <c r="G38" s="129"/>
-      <c r="H38" s="129"/>
-      <c r="I38" s="130"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="120"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="120"/>
+      <c r="I38" s="121"/>
     </row>
     <row r="39" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B39" s="131"/>
-      <c r="C39" s="129"/>
-      <c r="D39" s="129"/>
-      <c r="E39" s="129"/>
-      <c r="F39" s="129"/>
-      <c r="G39" s="129"/>
-      <c r="H39" s="129"/>
-      <c r="I39" s="130"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="120"/>
+      <c r="F39" s="120"/>
+      <c r="G39" s="120"/>
+      <c r="H39" s="120"/>
+      <c r="I39" s="121"/>
     </row>
     <row r="40" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B40" s="131"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="129"/>
-      <c r="E40" s="129"/>
-      <c r="F40" s="129"/>
-      <c r="G40" s="129"/>
-      <c r="H40" s="129"/>
-      <c r="I40" s="130"/>
+      <c r="B40" s="122"/>
+      <c r="C40" s="120"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="120"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="121"/>
     </row>
     <row r="41" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B41" s="131"/>
-      <c r="C41" s="129"/>
-      <c r="D41" s="129"/>
-      <c r="E41" s="129"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="129"/>
-      <c r="H41" s="129"/>
-      <c r="I41" s="130"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="121"/>
     </row>
     <row r="42" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B42" s="132"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="133"/>
-      <c r="I42" s="134"/>
+      <c r="B42" s="123"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="124"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="124"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="124"/>
+      <c r="I42" s="125"/>
     </row>
     <row r="43" spans="2:9" ht="16.5" customHeight="1">
       <c r="B43" s="5" t="s">
@@ -20667,54 +20686,38 @@
     <row r="1008" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I42"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="H19:I19"/>
@@ -20731,38 +20734,54 @@
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I42"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -20771,25 +20790,25 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="B1:H978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="20.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -21024,15 +21043,15 @@
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="17" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B17" s="115" t="s">
+      <c r="B17" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
-      <c r="H17" s="127"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="118"/>
     </row>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
       <c r="B18" s="160"/>
@@ -22039,25 +22058,25 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="B1:H998"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="14.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -22351,15 +22370,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="127"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="160" t="s">
@@ -23386,25 +23405,25 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="17" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -23730,15 +23749,15 @@
     </row>
     <row r="20" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="127"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="118"/>
     </row>
     <row r="22" spans="2:8" ht="21.75" customHeight="1">
       <c r="B22" s="160" t="s">
@@ -24759,25 +24778,25 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="B1:H997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="14.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -24977,11 +24996,19 @@
       <c r="H12" s="59"/>
     </row>
     <row r="13" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B13" s="55"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="55" t="s">
+        <v>592</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>593</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="45"/>
+      <c r="F13" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="G13" s="34"/>
       <c r="H13" s="48"/>
     </row>
@@ -25014,15 +25041,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="160"/>
@@ -26041,25 +26068,25 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="B1:H997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -26310,15 +26337,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="160" t="s">
@@ -27339,25 +27366,25 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="B1:H998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="17.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -27635,15 +27662,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="127"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="118"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="160"/>
@@ -28662,25 +28689,25 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="B1:H999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="17.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -28935,15 +28962,15 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="127"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="118"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="160"/>
@@ -29962,25 +29989,25 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="B1:H1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="17.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -30261,15 +30288,15 @@
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="22" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="126"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="127"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="118"/>
     </row>
     <row r="23" spans="2:8" ht="21.75" customHeight="1">
       <c r="B23" s="160"/>
@@ -31288,25 +31315,25 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="B1:H990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="17.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -31418,15 +31445,15 @@
     </row>
     <row r="10" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="11" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="126"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
-      <c r="H11" s="127"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="118"/>
     </row>
     <row r="12" spans="2:8" ht="21.75" customHeight="1">
       <c r="B12" s="160"/>
@@ -32445,25 +32472,25 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="B1:H997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="2" width="15.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -32638,15 +32665,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="118"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="160"/>
@@ -33671,29 +33698,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="156" t="s">
         <v>538</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34118,15 +34145,15 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="127"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="118"/>
     </row>
     <row r="29" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B29" s="160" t="s">
@@ -34172,29 +34199,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="156" t="s">
         <v>525</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34394,15 +34421,15 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="127"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="118"/>
     </row>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B22" s="26"/>
@@ -34442,29 +34469,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="156" t="s">
         <v>417</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34682,15 +34709,15 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="127"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="118"/>
     </row>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B22" s="26"/>
@@ -34730,32 +34757,32 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:H985"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
-    <col min="2" max="3" width="14.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="2" max="3" width="14.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="156" t="s">
         <v>527</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
@@ -34999,15 +35026,15 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="127"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="118"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="26"/>
@@ -41732,23 +41759,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="5" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="18.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
+    <col min="7" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -42936,23 +42963,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:H991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="5" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="3" width="18.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
+    <col min="7" max="8" width="12.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -44132,24 +44159,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:H997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" style="5" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="5" customWidth="1"/>
-    <col min="9" max="25" width="7.5703125" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="14.42578125" style="5"/>
+    <col min="3" max="4" width="12.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="5" customWidth="1"/>
+    <col min="9" max="25" width="7.5546875" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
@@ -44385,12 +44412,12 @@
       <c r="B18" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="113"/>
-      <c r="H18" s="114"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="115"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="160" t="s">

</xml_diff>

<commit_message>
2023/03/27 서정현/ DB 수정
</commit_message>
<xml_diff>
--- a/DB/LeMo 테이블 명세서 v1.0.xlsx
+++ b/DB/LeMo 테이블 명세서 v1.0.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="612">
   <si>
     <t>작업일자</t>
   </si>
@@ -3053,6 +3053,10 @@
   </si>
   <si>
     <t>lemo__product_coupon(상품 쿠폰) &gt; acc_id null 허용으로 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemo_product_review(리뷰) &gt; revi_reply_rdate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4338,10 +4342,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4350,20 +4357,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -4376,21 +4422,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4437,35 +4468,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4478,51 +4527,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4811,339 +4815,339 @@
   <sheetData>
     <row r="1" spans="2:9" ht="4.5" customHeight="1"/>
     <row r="2" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="134"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108"/>
       <c r="F2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="138" t="s">
+      <c r="G2" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="139"/>
-      <c r="I2" s="115"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="114"/>
     </row>
     <row r="3" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B3" s="135"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="111"/>
       <c r="F3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="138" t="s">
+      <c r="G3" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="139"/>
-      <c r="I3" s="115"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
     </row>
     <row r="4" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="138" t="s">
+      <c r="C4" s="114"/>
+      <c r="D4" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="115"/>
+      <c r="E4" s="114"/>
       <c r="F4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="140">
+      <c r="G4" s="116">
         <v>44982</v>
       </c>
-      <c r="H4" s="139"/>
-      <c r="I4" s="115"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="114"/>
     </row>
     <row r="5" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="138" t="s">
+      <c r="C5" s="114"/>
+      <c r="D5" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="115"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="138" t="s">
+      <c r="G5" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="139"/>
-      <c r="I5" s="115"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="114"/>
     </row>
     <row r="6" spans="2:9" ht="6" customHeight="1"/>
     <row r="7" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="114" t="s">
+      <c r="C7" s="113"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="139"/>
-      <c r="G7" s="141"/>
-      <c r="H7" s="114" t="s">
+      <c r="F7" s="113"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="115"/>
+      <c r="I7" s="114"/>
     </row>
     <row r="8" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="122" t="s">
         <v>376</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="111" t="s">
+      <c r="C8" s="123"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="125" t="s">
         <v>548</v>
       </c>
-      <c r="F8" s="109"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="113"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="105"/>
     </row>
     <row r="9" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="122" t="s">
         <v>547</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="111" t="s">
+      <c r="C9" s="123"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="125" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="109"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="113"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="105"/>
     </row>
     <row r="10" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="103" t="s">
+      <c r="C10" s="118"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="105"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="100"/>
     </row>
     <row r="11" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103" t="s">
+      <c r="C11" s="102"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="105"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="100"/>
     </row>
     <row r="12" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="117" t="s">
         <v>509</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="103" t="s">
+      <c r="C12" s="118"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="105"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="100"/>
     </row>
     <row r="13" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="117" t="s">
         <v>510</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="103" t="s">
+      <c r="C13" s="118"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="101" t="s">
         <v>511</v>
       </c>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="105"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="100"/>
     </row>
     <row r="14" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103" t="s">
+      <c r="C14" s="102"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="105"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="100"/>
     </row>
     <row r="15" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="117" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103" t="s">
+      <c r="C15" s="102"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="105"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="100"/>
     </row>
     <row r="16" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="117" t="s">
         <v>248</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="103" t="s">
+      <c r="C16" s="102"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="105"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="100"/>
     </row>
     <row r="17" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="117" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="103" t="s">
+      <c r="C17" s="102"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="101" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="101"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="105"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="100"/>
     </row>
     <row r="18" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B18" s="100" t="s">
+      <c r="B18" s="117" t="s">
         <v>250</v>
       </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103" t="s">
+      <c r="C18" s="102"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="F18" s="101"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="105"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="100"/>
     </row>
     <row r="19" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="117" t="s">
         <v>467</v>
       </c>
-      <c r="C19" s="101"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="103" t="s">
+      <c r="C19" s="102"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="101" t="s">
         <v>466</v>
       </c>
-      <c r="F19" s="101"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="105"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="100"/>
     </row>
     <row r="20" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B20" s="100" t="s">
+      <c r="B20" s="117" t="s">
         <v>471</v>
       </c>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="103" t="s">
+      <c r="C20" s="102"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="101" t="s">
         <v>470</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="105"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="100"/>
     </row>
     <row r="21" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="117" t="s">
         <v>409</v>
       </c>
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="103" t="s">
+      <c r="C21" s="102"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="101" t="s">
         <v>455</v>
       </c>
-      <c r="F21" s="101"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="105"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="100"/>
     </row>
     <row r="22" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="117" t="s">
         <v>460</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="103" t="s">
+      <c r="C22" s="102"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="101" t="s">
         <v>461</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="105"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="100"/>
     </row>
     <row r="23" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="117" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="101"/>
-      <c r="D23" s="102"/>
-      <c r="E23" s="103" t="s">
+      <c r="C23" s="102"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="F23" s="101"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="105"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="100"/>
     </row>
     <row r="24" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="117" t="s">
         <v>378</v>
       </c>
-      <c r="C24" s="101"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="103" t="s">
+      <c r="C24" s="102"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="101" t="s">
         <v>379</v>
       </c>
-      <c r="F24" s="101"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="105"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="100"/>
     </row>
     <row r="25" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="117" t="s">
         <v>323</v>
       </c>
-      <c r="C25" s="101"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="103" t="s">
+      <c r="C25" s="102"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="101" t="s">
         <v>377</v>
       </c>
-      <c r="F25" s="101"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="104"/>
-      <c r="I25" s="105"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="100"/>
     </row>
     <row r="26" spans="2:9" ht="21.75" customHeight="1">
       <c r="B26" s="82" t="s">
@@ -5151,241 +5155,241 @@
       </c>
       <c r="C26" s="83"/>
       <c r="D26" s="84"/>
-      <c r="E26" s="103" t="s">
+      <c r="E26" s="101" t="s">
         <v>380</v>
       </c>
-      <c r="F26" s="101"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="105"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="100"/>
     </row>
     <row r="27" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B27" s="100" t="s">
+      <c r="B27" s="117" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="101"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="103" t="s">
+      <c r="C27" s="102"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="101" t="s">
         <v>252</v>
       </c>
-      <c r="F27" s="101"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="105"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="100"/>
     </row>
     <row r="28" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="117" t="s">
         <v>383</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="102"/>
-      <c r="E28" s="103" t="s">
+      <c r="C28" s="102"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="101" t="s">
         <v>382</v>
       </c>
-      <c r="F28" s="101"/>
-      <c r="G28" s="102"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="105"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="100"/>
     </row>
     <row r="29" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B29" s="100" t="s">
+      <c r="B29" s="117" t="s">
         <v>325</v>
       </c>
-      <c r="C29" s="101"/>
-      <c r="D29" s="102"/>
-      <c r="E29" s="103" t="s">
+      <c r="C29" s="102"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="F29" s="101"/>
-      <c r="G29" s="102"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="105"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
     </row>
     <row r="30" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="117" t="s">
         <v>387</v>
       </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="102"/>
-      <c r="E30" s="103" t="s">
+      <c r="C30" s="102"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="101" t="s">
         <v>386</v>
       </c>
-      <c r="F30" s="101"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="105"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="100"/>
     </row>
     <row r="31" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="117" t="s">
         <v>404</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="103" t="s">
+      <c r="C31" s="102"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="101" t="s">
         <v>403</v>
       </c>
-      <c r="F31" s="101"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="104"/>
-      <c r="I31" s="105"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="100"/>
     </row>
     <row r="32" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="117" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="106"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="103" t="s">
+      <c r="C32" s="118"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="101" t="s">
         <v>389</v>
       </c>
-      <c r="F32" s="106"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="105"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="119"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="100"/>
     </row>
     <row r="33" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="117" t="s">
         <v>390</v>
       </c>
-      <c r="C33" s="106"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="103" t="s">
+      <c r="C33" s="118"/>
+      <c r="D33" s="119"/>
+      <c r="E33" s="101" t="s">
         <v>391</v>
       </c>
-      <c r="F33" s="106"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="104"/>
-      <c r="I33" s="105"/>
-      <c r="N33" s="99"/>
-      <c r="O33" s="99"/>
-      <c r="P33" s="99"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="100"/>
+      <c r="N33" s="141"/>
+      <c r="O33" s="141"/>
+      <c r="P33" s="141"/>
     </row>
     <row r="34" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B34" s="100" t="s">
+      <c r="B34" s="117" t="s">
         <v>392</v>
       </c>
-      <c r="C34" s="106"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="103" t="s">
+      <c r="C34" s="118"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="101" t="s">
         <v>393</v>
       </c>
-      <c r="F34" s="106"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="104"/>
-      <c r="I34" s="105"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="100"/>
     </row>
     <row r="35" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B35" s="100"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="105"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="101"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="119"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="100"/>
     </row>
     <row r="36" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B36" s="100"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="105"/>
+      <c r="B36" s="117"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="119"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="100"/>
     </row>
     <row r="37" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B37" s="131"/>
-      <c r="C37" s="127"/>
-      <c r="D37" s="128"/>
-      <c r="E37" s="126"/>
-      <c r="F37" s="127"/>
-      <c r="G37" s="128"/>
-      <c r="H37" s="129"/>
-      <c r="I37" s="130"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="136"/>
+      <c r="D37" s="137"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="137"/>
+      <c r="H37" s="138"/>
+      <c r="I37" s="139"/>
     </row>
     <row r="38" spans="2:16" ht="6" customHeight="1"/>
     <row r="39" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="117"/>
-      <c r="D39" s="117"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="117"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="117"/>
-      <c r="I39" s="118"/>
+      <c r="C39" s="126"/>
+      <c r="D39" s="126"/>
+      <c r="E39" s="126"/>
+      <c r="F39" s="126"/>
+      <c r="G39" s="126"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="127"/>
     </row>
     <row r="40" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B40" s="119"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="120"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="121"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="129"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="130"/>
     </row>
     <row r="41" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B41" s="122"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="121"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="129"/>
+      <c r="H41" s="129"/>
+      <c r="I41" s="130"/>
     </row>
     <row r="42" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B42" s="122"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="120"/>
-      <c r="G42" s="120"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="121"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="129"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="129"/>
+      <c r="H42" s="129"/>
+      <c r="I42" s="130"/>
     </row>
     <row r="43" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B43" s="122"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="120"/>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="121"/>
+      <c r="B43" s="131"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="130"/>
     </row>
     <row r="44" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B44" s="122"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="121"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="129"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="129"/>
+      <c r="I44" s="130"/>
     </row>
     <row r="45" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B45" s="122"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="121"/>
+      <c r="B45" s="131"/>
+      <c r="C45" s="129"/>
+      <c r="D45" s="129"/>
+      <c r="E45" s="129"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="129"/>
+      <c r="H45" s="129"/>
+      <c r="I45" s="130"/>
     </row>
     <row r="46" spans="2:16" ht="16.5" customHeight="1">
-      <c r="B46" s="123"/>
-      <c r="C46" s="124"/>
-      <c r="D46" s="124"/>
-      <c r="E46" s="124"/>
-      <c r="F46" s="124"/>
-      <c r="G46" s="124"/>
-      <c r="H46" s="124"/>
-      <c r="I46" s="125"/>
+      <c r="B46" s="132"/>
+      <c r="C46" s="133"/>
+      <c r="D46" s="133"/>
+      <c r="E46" s="133"/>
+      <c r="F46" s="133"/>
+      <c r="G46" s="133"/>
+      <c r="H46" s="133"/>
+      <c r="I46" s="134"/>
     </row>
     <row r="47" spans="2:16" ht="16.5" customHeight="1">
       <c r="B47" s="5" t="s">
@@ -6359,15 +6363,77 @@
     <row r="1012" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N33:P33"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B40:I46"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
@@ -6392,77 +6458,15 @@
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B40:I46"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -6725,15 +6729,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="161"/>
@@ -8128,12 +8132,12 @@
       <c r="B22" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="139"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="115"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="114"/>
     </row>
     <row r="23" spans="2:8" ht="21.75" customHeight="1">
       <c r="B23" s="161" t="s">
@@ -9431,15 +9435,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="115" t="s">
         <v>254</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="161"/>
@@ -10926,15 +10930,15 @@
     </row>
     <row r="27" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="28" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="118"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="127"/>
     </row>
     <row r="29" spans="2:8" ht="21.75" customHeight="1">
       <c r="B29" s="26" t="s">
@@ -12143,15 +12147,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -13352,15 +13356,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -14559,15 +14563,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="26"/>
@@ -15769,15 +15773,15 @@
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="17" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="118"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="127"/>
     </row>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
       <c r="B18" s="26"/>
@@ -16965,15 +16969,15 @@
     </row>
     <row r="12" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="13" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="118"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="127"/>
     </row>
     <row r="14" spans="2:8" ht="21.75" customHeight="1">
       <c r="B14" s="26"/>
@@ -18276,15 +18280,15 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="116" t="s">
+      <c r="B20" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="117"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="118"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="126"/>
+      <c r="H20" s="127"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="161" t="s">
@@ -19297,7 +19301,7 @@
   <dimension ref="B1:P1008"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -19315,503 +19319,509 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="145" t="s">
         <v>562</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
     </row>
     <row r="2" spans="2:9" ht="6" customHeight="1"/>
     <row r="3" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="115" t="s">
         <v>563</v>
       </c>
-      <c r="C3" s="139"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="114" t="s">
+      <c r="C3" s="113"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="139"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="114" t="s">
+      <c r="F3" s="113"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="121" t="s">
         <v>564</v>
       </c>
-      <c r="I3" s="115"/>
+      <c r="I3" s="114"/>
     </row>
     <row r="4" spans="2:9" ht="42.6" customHeight="1">
-      <c r="B4" s="142">
+      <c r="B4" s="157">
         <v>1</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="145" t="s">
+      <c r="C4" s="158"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="160" t="s">
         <v>565</v>
       </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="146">
+      <c r="F4" s="123"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="155">
         <v>44999</v>
       </c>
-      <c r="I4" s="147"/>
+      <c r="I4" s="156"/>
     </row>
     <row r="5" spans="2:9" ht="41.25" customHeight="1">
-      <c r="B5" s="142">
+      <c r="B5" s="157">
         <v>2</v>
       </c>
-      <c r="C5" s="143"/>
-      <c r="D5" s="144"/>
-      <c r="E5" s="145" t="s">
+      <c r="C5" s="158"/>
+      <c r="D5" s="159"/>
+      <c r="E5" s="160" t="s">
         <v>567</v>
       </c>
-      <c r="F5" s="109"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="146">
+      <c r="F5" s="123"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="155">
         <v>44999</v>
       </c>
-      <c r="I5" s="147"/>
+      <c r="I5" s="156"/>
     </row>
     <row r="6" spans="2:9" ht="44.45" customHeight="1">
-      <c r="B6" s="148">
+      <c r="B6" s="146">
         <v>3</v>
       </c>
-      <c r="C6" s="149"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="151" t="s">
+      <c r="C6" s="147"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="154" t="s">
         <v>569</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="146">
+      <c r="F6" s="102"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="155">
         <v>45001</v>
       </c>
-      <c r="I6" s="147"/>
+      <c r="I6" s="156"/>
     </row>
     <row r="7" spans="2:9" ht="69" customHeight="1">
-      <c r="B7" s="148">
+      <c r="B7" s="146">
         <v>4</v>
       </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="151" t="s">
+      <c r="C7" s="149"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="154" t="s">
         <v>575</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="146">
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="155">
         <v>45001</v>
       </c>
-      <c r="I7" s="147"/>
+      <c r="I7" s="156"/>
     </row>
     <row r="8" spans="2:9" ht="39.6" customHeight="1">
-      <c r="B8" s="148">
+      <c r="B8" s="146">
         <v>5</v>
       </c>
-      <c r="C8" s="149"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="151" t="s">
+      <c r="C8" s="147"/>
+      <c r="D8" s="148"/>
+      <c r="E8" s="154" t="s">
         <v>576</v>
       </c>
-      <c r="F8" s="106"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="154">
+      <c r="F8" s="118"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="151">
         <v>45002</v>
       </c>
-      <c r="I8" s="155"/>
+      <c r="I8" s="153"/>
     </row>
     <row r="9" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B9" s="148">
+      <c r="B9" s="146">
         <v>6</v>
       </c>
-      <c r="C9" s="149"/>
-      <c r="D9" s="150"/>
-      <c r="E9" s="103" t="s">
+      <c r="C9" s="147"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="101" t="s">
         <v>577</v>
       </c>
-      <c r="F9" s="106"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="154">
+      <c r="F9" s="118"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="151">
         <v>45003</v>
       </c>
-      <c r="I9" s="155"/>
+      <c r="I9" s="153"/>
     </row>
     <row r="10" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B10" s="148">
+      <c r="B10" s="146">
         <v>7</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="103" t="s">
+      <c r="C10" s="149"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="101" t="s">
         <v>578</v>
       </c>
-      <c r="F10" s="106"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="154">
+      <c r="F10" s="118"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="151">
         <v>45005</v>
       </c>
-      <c r="I10" s="155"/>
+      <c r="I10" s="153"/>
     </row>
     <row r="11" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B11" s="148">
+      <c r="B11" s="146">
         <v>8</v>
       </c>
-      <c r="C11" s="152"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="103" t="s">
+      <c r="C11" s="149"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="101" t="s">
         <v>583</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="154">
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="151">
         <v>45006</v>
       </c>
-      <c r="I11" s="155"/>
+      <c r="I11" s="153"/>
     </row>
     <row r="12" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B12" s="148">
+      <c r="B12" s="146">
         <v>9</v>
       </c>
-      <c r="C12" s="152"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="103" t="s">
+      <c r="C12" s="149"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="101" t="s">
         <v>584</v>
       </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="154">
+      <c r="F12" s="102"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="151">
         <v>45006</v>
       </c>
-      <c r="I12" s="155"/>
+      <c r="I12" s="153"/>
     </row>
     <row r="13" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B13" s="148">
+      <c r="B13" s="146">
         <v>10</v>
       </c>
-      <c r="C13" s="152"/>
-      <c r="D13" s="153"/>
-      <c r="E13" s="103" t="s">
+      <c r="C13" s="149"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="101" t="s">
         <v>586</v>
       </c>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="154">
+      <c r="F13" s="102"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="151">
         <v>45006</v>
       </c>
-      <c r="I13" s="155"/>
+      <c r="I13" s="153"/>
     </row>
     <row r="14" spans="2:9" ht="38.25" customHeight="1">
-      <c r="B14" s="148">
+      <c r="B14" s="146">
         <v>11</v>
       </c>
-      <c r="C14" s="152"/>
-      <c r="D14" s="153"/>
-      <c r="E14" s="151" t="s">
+      <c r="C14" s="149"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="154" t="s">
         <v>587</v>
       </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="154">
+      <c r="F14" s="102"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="151">
         <v>45007</v>
       </c>
-      <c r="I14" s="155"/>
+      <c r="I14" s="153"/>
     </row>
     <row r="15" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B15" s="148">
+      <c r="B15" s="146">
         <v>12</v>
       </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="103" t="s">
+      <c r="C15" s="149"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="101" t="s">
         <v>603</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="154">
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="151">
         <v>45007</v>
       </c>
-      <c r="I15" s="155"/>
+      <c r="I15" s="153"/>
     </row>
     <row r="16" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B16" s="148">
+      <c r="B16" s="146">
         <v>13</v>
       </c>
-      <c r="C16" s="152"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="103" t="s">
+      <c r="C16" s="149"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="101" t="s">
         <v>602</v>
       </c>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="154">
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="151">
         <v>45008</v>
       </c>
-      <c r="I16" s="156"/>
+      <c r="I16" s="152"/>
     </row>
     <row r="17" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B17" s="148">
+      <c r="B17" s="146">
         <v>14</v>
       </c>
-      <c r="C17" s="152"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="103" t="s">
+      <c r="C17" s="149"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="101" t="s">
         <v>610</v>
       </c>
-      <c r="F17" s="101"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="154">
+      <c r="F17" s="102"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="151">
         <v>45009</v>
       </c>
-      <c r="I17" s="156"/>
+      <c r="I17" s="152"/>
     </row>
     <row r="18" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B18" s="148"/>
-      <c r="C18" s="152"/>
-      <c r="D18" s="153"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="105"/>
+      <c r="B18" s="146">
+        <v>15</v>
+      </c>
+      <c r="C18" s="149"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="101" t="s">
+        <v>611</v>
+      </c>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="151">
+        <v>45012</v>
+      </c>
+      <c r="I18" s="152"/>
     </row>
     <row r="19" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B19" s="148"/>
-      <c r="C19" s="152"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="105"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="100"/>
     </row>
     <row r="20" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B20" s="148"/>
-      <c r="C20" s="152"/>
-      <c r="D20" s="153"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="105"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="100"/>
     </row>
     <row r="21" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B21" s="148"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="105"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="150"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="100"/>
     </row>
     <row r="22" spans="2:16" ht="21.75" customHeight="1">
       <c r="B22" s="97"/>
       <c r="C22" s="94"/>
       <c r="D22" s="56"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="105"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="100"/>
     </row>
     <row r="23" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B23" s="148"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="105"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="149"/>
+      <c r="D23" s="150"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="100"/>
     </row>
     <row r="24" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B24" s="148"/>
-      <c r="C24" s="152"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="105"/>
+      <c r="B24" s="146"/>
+      <c r="C24" s="149"/>
+      <c r="D24" s="150"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="100"/>
     </row>
     <row r="25" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B25" s="148"/>
-      <c r="C25" s="152"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="104"/>
-      <c r="I25" s="105"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="100"/>
     </row>
     <row r="26" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B26" s="148"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="153"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="105"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="150"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="100"/>
     </row>
     <row r="27" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B27" s="148"/>
-      <c r="C27" s="152"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="105"/>
+      <c r="B27" s="146"/>
+      <c r="C27" s="149"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="100"/>
     </row>
     <row r="28" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B28" s="148"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="105"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="100"/>
     </row>
     <row r="29" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="105"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
+      <c r="B29" s="146"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="119"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="100"/>
+      <c r="N29" s="141"/>
+      <c r="O29" s="141"/>
+      <c r="P29" s="141"/>
     </row>
     <row r="30" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B30" s="148"/>
-      <c r="C30" s="149"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="107"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="105"/>
+      <c r="B30" s="146"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="119"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="100"/>
     </row>
     <row r="31" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="104"/>
-      <c r="I31" s="105"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="147"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="119"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="100"/>
     </row>
     <row r="32" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B32" s="148"/>
-      <c r="C32" s="149"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="105"/>
+      <c r="B32" s="146"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="119"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="100"/>
     </row>
     <row r="33" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B33" s="158"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="160"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="128"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="130"/>
+      <c r="B33" s="142"/>
+      <c r="C33" s="143"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="135"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="139"/>
     </row>
     <row r="34" spans="2:9" ht="6" customHeight="1"/>
     <row r="35" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B35" s="116" t="s">
+      <c r="B35" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="117"/>
-      <c r="I35" s="118"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="126"/>
+      <c r="H35" s="126"/>
+      <c r="I35" s="127"/>
     </row>
     <row r="36" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B36" s="119"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="120"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="120"/>
-      <c r="I36" s="121"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="129"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="130"/>
     </row>
     <row r="37" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B37" s="122"/>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="120"/>
-      <c r="G37" s="120"/>
-      <c r="H37" s="120"/>
-      <c r="I37" s="121"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="129"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="129"/>
+      <c r="F37" s="129"/>
+      <c r="G37" s="129"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="130"/>
     </row>
     <row r="38" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B38" s="122"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="120"/>
-      <c r="G38" s="120"/>
-      <c r="H38" s="120"/>
-      <c r="I38" s="121"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="129"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="129"/>
+      <c r="F38" s="129"/>
+      <c r="G38" s="129"/>
+      <c r="H38" s="129"/>
+      <c r="I38" s="130"/>
     </row>
     <row r="39" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B39" s="122"/>
-      <c r="C39" s="120"/>
-      <c r="D39" s="120"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="120"/>
-      <c r="G39" s="120"/>
-      <c r="H39" s="120"/>
-      <c r="I39" s="121"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="129"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="129"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="129"/>
+      <c r="H39" s="129"/>
+      <c r="I39" s="130"/>
     </row>
     <row r="40" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B40" s="122"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="120"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="121"/>
+      <c r="B40" s="131"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="129"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="130"/>
     </row>
     <row r="41" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B41" s="122"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="121"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="129"/>
+      <c r="H41" s="129"/>
+      <c r="I41" s="130"/>
     </row>
     <row r="42" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B42" s="123"/>
-      <c r="C42" s="124"/>
-      <c r="D42" s="124"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="124"/>
-      <c r="G42" s="124"/>
-      <c r="H42" s="124"/>
-      <c r="I42" s="125"/>
+      <c r="B42" s="132"/>
+      <c r="C42" s="133"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="133"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="133"/>
+      <c r="H42" s="133"/>
+      <c r="I42" s="134"/>
     </row>
     <row r="43" spans="2:9" ht="16.5" customHeight="1">
       <c r="B43" s="5" t="s">
@@ -20785,11 +20795,81 @@
     <row r="1008" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I42"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
@@ -20806,81 +20886,11 @@
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -21142,15 +21152,15 @@
     </row>
     <row r="16" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="17" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="118"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="127"/>
     </row>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
       <c r="B18" s="161"/>
@@ -22469,15 +22479,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="161" t="s">
@@ -23848,15 +23858,15 @@
     </row>
     <row r="20" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B21" s="116" t="s">
+      <c r="B21" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="118"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="126"/>
+      <c r="H21" s="127"/>
     </row>
     <row r="22" spans="2:8" ht="21.75" customHeight="1">
       <c r="B22" s="161" t="s">
@@ -25157,15 +25167,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="161"/>
@@ -26453,15 +26463,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="161" t="s">
@@ -27778,15 +27788,15 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="127"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
       <c r="B20" s="161"/>
@@ -29088,15 +29098,15 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="116" t="s">
+      <c r="B20" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="117"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="118"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="126"/>
+      <c r="H20" s="127"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="161"/>
@@ -30414,15 +30424,15 @@
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="22" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="118"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
+      <c r="G22" s="126"/>
+      <c r="H22" s="127"/>
     </row>
     <row r="23" spans="2:8" ht="21.75" customHeight="1">
       <c r="B23" s="161"/>
@@ -31634,15 +31644,15 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="18" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="118"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="127"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="161"/>
@@ -32797,15 +32807,15 @@
     </row>
     <row r="10" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="11" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="117"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="118"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="127"/>
     </row>
     <row r="12" spans="2:8" ht="21.75" customHeight="1">
       <c r="B12" s="161"/>
@@ -33842,11 +33852,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="145" t="s">
         <v>532</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34271,15 +34281,15 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="118"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="127"/>
     </row>
     <row r="29" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B29" s="161" t="s">
@@ -34343,11 +34353,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="145" t="s">
         <v>519</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34555,15 +34565,15 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B21" s="116" t="s">
+      <c r="B21" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="118"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="126"/>
+      <c r="H21" s="127"/>
     </row>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B22" s="26"/>
@@ -34621,11 +34631,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="145" t="s">
         <v>411</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -34843,15 +34853,15 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B21" s="116" t="s">
+      <c r="B21" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="118"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="126"/>
+      <c r="H21" s="127"/>
     </row>
     <row r="22" spans="2:8" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="B22" s="26"/>
@@ -34912,11 +34922,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="145" t="s">
         <v>521</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:8" ht="16.5" customHeight="1">
@@ -35160,15 +35170,15 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:8" ht="21.75" customHeight="1">
-      <c r="B20" s="116" t="s">
+      <c r="B20" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="117"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="118"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="126"/>
+      <c r="H20" s="127"/>
     </row>
     <row r="21" spans="2:8" ht="21.75" customHeight="1">
       <c r="B21" s="26"/>
@@ -44546,12 +44556,12 @@
       <c r="B18" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="139"/>
-      <c r="D18" s="139"/>
-      <c r="E18" s="139"/>
-      <c r="F18" s="139"/>
-      <c r="G18" s="139"/>
-      <c r="H18" s="115"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="114"/>
     </row>
     <row r="19" spans="2:8" ht="21.75" customHeight="1">
       <c r="B19" s="161" t="s">

</xml_diff>